<commit_message>
#2: preparing for update
</commit_message>
<xml_diff>
--- a/materials/experiment.xlsx
+++ b/materials/experiment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="testtrials" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="102">
   <si>
     <t xml:space="preserve">screwdriver</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">pen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">igp1</t>
   </si>
   <si>
     <t xml:space="preserve">bigblock (D)</t>
@@ -455,10 +458,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,6 +498,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -521,39 +529,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -582,94 +590,150 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -684,12 +748,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -699,95 +763,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -816,71 +824,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -888,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,60 +904,60 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -957,20 +965,20 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -999,39 +1007,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1060,39 +1068,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1124,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,28 +1140,28 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1182,31 +1190,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -1214,7 +1222,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1243,31 +1251,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -1275,7 +1283,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1307,10 +1315,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,25 +1326,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1368,10 +1376,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1379,25 +1387,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1426,39 +1434,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1487,34 +1495,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,28 +1562,28 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1604,15 +1612,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -1620,15 +1628,15 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>0</v>
@@ -1636,7 +1644,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1665,15 +1673,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -1681,23 +1689,23 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1718,7 +1726,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1726,15 +1734,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,23 +1750,23 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1787,15 +1795,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,23 +1811,23 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1848,100 +1856,100 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>